<commit_message>
date format, customer details changes,sopc duplicate avoid
</commit_message>
<xml_diff>
--- a/public/assets/files/Customers_Demo_File.xlsx
+++ b/public/assets/files/Customers_Demo_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\jisha\TripleFast\public\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOMSHER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1A549-8816-46D2-88C4-5B5676988E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D3CEF8D-0261-4BF3-8BBB-C6E06D08440F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3884E6A6-979B-4C92-AE74-32409635477F}"/>
   </bookViews>
@@ -34,18 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Customer ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email </t>
   </si>
   <si>
     <r>
@@ -78,6 +69,25 @@
       </rPr>
       <t>(Optional)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Optional)</t>
+    </r>
+  </si>
+  <si>
+    <t>Customer Name</t>
   </si>
 </sst>
 </file>
@@ -457,46 +467,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795A7C93-5BFE-4022-8DF0-CAC14BE7451D}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="2"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -504,9 +510,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -514,9 +519,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -524,9 +528,8 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -534,9 +537,8 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -544,9 +546,8 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -554,9 +555,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -564,9 +564,8 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -574,9 +573,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -584,9 +582,8 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -594,9 +591,8 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -604,9 +600,8 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -614,9 +609,8 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -624,9 +618,8 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -634,9 +627,8 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -644,9 +636,8 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -654,9 +645,8 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -664,9 +654,8 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -674,9 +663,8 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -684,9 +672,8 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -694,9 +681,8 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -704,9 +690,8 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -714,9 +699,8 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -724,9 +708,8 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -734,9 +717,8 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -744,9 +726,8 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -754,9 +735,8 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -764,9 +744,8 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -774,9 +753,8 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -784,9 +762,8 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -794,9 +771,8 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -804,9 +780,8 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -814,7 +789,6 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>